<commit_message>
/ ‘Extended Campuses/Self Appraisals/2016/TME Data Jan 2016 - June 2016.xlsx’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2016/TME Data Jan 2016 - June 2016.xlsx
+++ b/Extended Campuses/Self Appraisals/2016/TME Data Jan 2016 - June 2016.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$E$1:$F$485</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1645,7 +1648,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -1723,7 +1726,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -2020,10 +2023,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A471" workbookViewId="0">
-      <selection activeCell="H483" sqref="H483"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G217" sqref="G217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -2107,7 +2111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
@@ -2130,7 +2134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -2153,7 +2157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2176,7 +2180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2199,7 +2203,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2222,7 +2226,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2245,7 +2249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2268,7 +2272,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>6</v>
       </c>
@@ -2291,7 +2295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -2314,7 +2318,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -2337,7 +2341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -2383,7 +2387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -2406,7 +2410,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -2429,7 +2433,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -2452,7 +2456,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>6</v>
       </c>
@@ -2475,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -2498,7 +2502,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -2521,7 +2525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2567,7 +2571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -2590,7 +2594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -2613,7 +2617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -2636,7 +2640,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2682,7 +2686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6</v>
       </c>
@@ -2705,7 +2709,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -2728,7 +2732,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2751,7 +2755,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>6</v>
       </c>
@@ -2774,7 +2778,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>6</v>
       </c>
@@ -2797,7 +2801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>6</v>
       </c>
@@ -2820,7 +2824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
@@ -2843,7 +2847,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>6</v>
       </c>
@@ -2866,7 +2870,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -2889,7 +2893,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -2912,7 +2916,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6</v>
       </c>
@@ -2935,7 +2939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6</v>
       </c>
@@ -2958,7 +2962,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>6</v>
       </c>
@@ -2981,7 +2985,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -3004,7 +3008,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
@@ -3027,7 +3031,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>6</v>
       </c>
@@ -3050,7 +3054,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>6</v>
       </c>
@@ -3073,7 +3077,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6</v>
       </c>
@@ -3096,7 +3100,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6</v>
       </c>
@@ -3119,7 +3123,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6</v>
       </c>
@@ -3142,7 +3146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>311</v>
       </c>
@@ -3165,7 +3169,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>311</v>
       </c>
@@ -3188,7 +3192,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>311</v>
       </c>
@@ -3211,7 +3215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>299</v>
       </c>
@@ -3234,7 +3238,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>299</v>
       </c>
@@ -3257,7 +3261,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>299</v>
       </c>
@@ -3280,7 +3284,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>299</v>
       </c>
@@ -3303,7 +3307,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>299</v>
       </c>
@@ -3326,7 +3330,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>299</v>
       </c>
@@ -3349,7 +3353,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>299</v>
       </c>
@@ -3372,7 +3376,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>299</v>
       </c>
@@ -3395,7 +3399,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>299</v>
       </c>
@@ -3418,7 +3422,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>299</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>299</v>
       </c>
@@ -3464,7 +3468,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>299</v>
       </c>
@@ -3487,7 +3491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>299</v>
       </c>
@@ -3510,7 +3514,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>299</v>
       </c>
@@ -3533,7 +3537,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>299</v>
       </c>
@@ -3556,7 +3560,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>299</v>
       </c>
@@ -3579,7 +3583,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>299</v>
       </c>
@@ -3602,7 +3606,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>299</v>
       </c>
@@ -3625,7 +3629,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>299</v>
       </c>
@@ -3648,7 +3652,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>299</v>
       </c>
@@ -3671,7 +3675,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>299</v>
       </c>
@@ -3694,7 +3698,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>299</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>299</v>
       </c>
@@ -3740,7 +3744,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>299</v>
       </c>
@@ -3763,7 +3767,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>299</v>
       </c>
@@ -3786,7 +3790,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>299</v>
       </c>
@@ -3809,7 +3813,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>299</v>
       </c>
@@ -3832,7 +3836,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>299</v>
       </c>
@@ -3855,7 +3859,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>299</v>
       </c>
@@ -3878,7 +3882,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>299</v>
       </c>
@@ -3901,7 +3905,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>299</v>
       </c>
@@ -3924,7 +3928,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>299</v>
       </c>
@@ -3947,7 +3951,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>299</v>
       </c>
@@ -3970,7 +3974,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>299</v>
       </c>
@@ -3993,7 +3997,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>299</v>
       </c>
@@ -4016,7 +4020,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>299</v>
       </c>
@@ -4039,7 +4043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>299</v>
       </c>
@@ -4062,7 +4066,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>299</v>
       </c>
@@ -4085,7 +4089,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>299</v>
       </c>
@@ -4108,7 +4112,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>299</v>
       </c>
@@ -4131,7 +4135,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>299</v>
       </c>
@@ -4154,7 +4158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>299</v>
       </c>
@@ -4177,7 +4181,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>299</v>
       </c>
@@ -4200,7 +4204,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>299</v>
       </c>
@@ -4223,7 +4227,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>299</v>
       </c>
@@ -4246,7 +4250,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>299</v>
       </c>
@@ -4269,7 +4273,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>299</v>
       </c>
@@ -4292,7 +4296,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>299</v>
       </c>
@@ -4315,7 +4319,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>299</v>
       </c>
@@ -4338,7 +4342,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>299</v>
       </c>
@@ -4361,7 +4365,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>299</v>
       </c>
@@ -4384,7 +4388,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>299</v>
       </c>
@@ -4407,7 +4411,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>299</v>
       </c>
@@ -4430,7 +4434,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>299</v>
       </c>
@@ -4453,7 +4457,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>299</v>
       </c>
@@ -4476,7 +4480,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>299</v>
       </c>
@@ -4499,7 +4503,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>299</v>
       </c>
@@ -4522,7 +4526,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>299</v>
       </c>
@@ -4545,7 +4549,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>299</v>
       </c>
@@ -4568,7 +4572,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>299</v>
       </c>
@@ -4591,7 +4595,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>299</v>
       </c>
@@ -4614,7 +4618,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>299</v>
       </c>
@@ -4637,7 +4641,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>299</v>
       </c>
@@ -4660,7 +4664,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>299</v>
       </c>
@@ -4683,7 +4687,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>299</v>
       </c>
@@ -4706,7 +4710,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>299</v>
       </c>
@@ -4729,7 +4733,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>299</v>
       </c>
@@ -4752,7 +4756,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>299</v>
       </c>
@@ -4775,7 +4779,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>299</v>
       </c>
@@ -4798,7 +4802,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>299</v>
       </c>
@@ -4821,7 +4825,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>299</v>
       </c>
@@ -4844,7 +4848,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>299</v>
       </c>
@@ -4867,7 +4871,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>299</v>
       </c>
@@ -4890,7 +4894,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>299</v>
       </c>
@@ -4913,7 +4917,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>299</v>
       </c>
@@ -4936,7 +4940,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>299</v>
       </c>
@@ -4959,7 +4963,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>299</v>
       </c>
@@ -4982,7 +4986,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>299</v>
       </c>
@@ -5005,7 +5009,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>299</v>
       </c>
@@ -5028,7 +5032,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>299</v>
       </c>
@@ -5051,7 +5055,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>299</v>
       </c>
@@ -5074,7 +5078,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>299</v>
       </c>
@@ -5097,7 +5101,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>299</v>
       </c>
@@ -5120,7 +5124,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>299</v>
       </c>
@@ -5143,7 +5147,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>299</v>
       </c>
@@ -5166,7 +5170,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>299</v>
       </c>
@@ -5189,7 +5193,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>299</v>
       </c>
@@ -5212,7 +5216,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>299</v>
       </c>
@@ -5235,7 +5239,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>299</v>
       </c>
@@ -5258,7 +5262,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>299</v>
       </c>
@@ -5281,7 +5285,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>299</v>
       </c>
@@ -5304,7 +5308,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>299</v>
       </c>
@@ -5327,7 +5331,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>299</v>
       </c>
@@ -5350,7 +5354,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>299</v>
       </c>
@@ -5373,7 +5377,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>299</v>
       </c>
@@ -5396,7 +5400,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>299</v>
       </c>
@@ -5419,7 +5423,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>299</v>
       </c>
@@ -5442,7 +5446,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>311</v>
       </c>
@@ -5465,7 +5469,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>311</v>
       </c>
@@ -5488,7 +5492,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>311</v>
       </c>
@@ -5511,7 +5515,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>311</v>
       </c>
@@ -5534,7 +5538,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>311</v>
       </c>
@@ -5557,7 +5561,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>311</v>
       </c>
@@ -5580,7 +5584,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>311</v>
       </c>
@@ -5603,7 +5607,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>311</v>
       </c>
@@ -5626,7 +5630,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>311</v>
       </c>
@@ -5649,7 +5653,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>299</v>
       </c>
@@ -5672,7 +5676,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>299</v>
       </c>
@@ -5695,7 +5699,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>299</v>
       </c>
@@ -5718,7 +5722,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>299</v>
       </c>
@@ -5741,7 +5745,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>299</v>
       </c>
@@ -5764,7 +5768,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>299</v>
       </c>
@@ -5787,7 +5791,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>299</v>
       </c>
@@ -5810,7 +5814,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>299</v>
       </c>
@@ -5833,7 +5837,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>299</v>
       </c>
@@ -5856,7 +5860,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>299</v>
       </c>
@@ -5879,7 +5883,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>299</v>
       </c>
@@ -5902,7 +5906,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>299</v>
       </c>
@@ -5925,7 +5929,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>299</v>
       </c>
@@ -5948,7 +5952,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>299</v>
       </c>
@@ -5971,7 +5975,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>299</v>
       </c>
@@ -5994,7 +5998,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>299</v>
       </c>
@@ -6017,7 +6021,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>299</v>
       </c>
@@ -6040,7 +6044,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>299</v>
       </c>
@@ -6063,7 +6067,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>299</v>
       </c>
@@ -6086,7 +6090,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="177" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>299</v>
       </c>
@@ -6109,7 +6113,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>299</v>
       </c>
@@ -6132,7 +6136,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>299</v>
       </c>
@@ -6155,7 +6159,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>299</v>
       </c>
@@ -6178,7 +6182,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>299</v>
       </c>
@@ -6201,7 +6205,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>299</v>
       </c>
@@ -6224,7 +6228,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>299</v>
       </c>
@@ -6247,7 +6251,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>299</v>
       </c>
@@ -6270,7 +6274,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>299</v>
       </c>
@@ -6293,7 +6297,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>299</v>
       </c>
@@ -6316,7 +6320,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>299</v>
       </c>
@@ -6339,7 +6343,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>299</v>
       </c>
@@ -6362,7 +6366,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>299</v>
       </c>
@@ -6385,7 +6389,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>299</v>
       </c>
@@ -6408,7 +6412,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>299</v>
       </c>
@@ -6431,7 +6435,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>299</v>
       </c>
@@ -6454,7 +6458,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>299</v>
       </c>
@@ -6477,7 +6481,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>299</v>
       </c>
@@ -6500,7 +6504,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>299</v>
       </c>
@@ -6523,7 +6527,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>299</v>
       </c>
@@ -6546,7 +6550,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>299</v>
       </c>
@@ -6569,7 +6573,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>299</v>
       </c>
@@ -6592,7 +6596,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>299</v>
       </c>
@@ -6615,7 +6619,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>299</v>
       </c>
@@ -6638,7 +6642,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>299</v>
       </c>
@@ -6661,7 +6665,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>299</v>
       </c>
@@ -6684,7 +6688,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>299</v>
       </c>
@@ -6707,7 +6711,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>299</v>
       </c>
@@ -6730,7 +6734,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>299</v>
       </c>
@@ -6753,7 +6757,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>299</v>
       </c>
@@ -6776,7 +6780,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>299</v>
       </c>
@@ -6799,7 +6803,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>349</v>
       </c>
@@ -6822,7 +6826,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>349</v>
       </c>
@@ -6845,7 +6849,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>349</v>
       </c>
@@ -6868,7 +6872,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>349</v>
       </c>
@@ -6891,7 +6895,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>349</v>
       </c>
@@ -6914,7 +6918,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>299</v>
       </c>
@@ -6937,7 +6941,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>299</v>
       </c>
@@ -6960,7 +6964,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>299</v>
       </c>
@@ -6983,7 +6987,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>299</v>
       </c>
@@ -7098,7 +7102,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>233</v>
       </c>
@@ -7121,7 +7125,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>233</v>
       </c>
@@ -7144,7 +7148,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>233</v>
       </c>
@@ -7167,7 +7171,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>233</v>
       </c>
@@ -7190,7 +7194,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>233</v>
       </c>
@@ -7213,7 +7217,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>233</v>
       </c>
@@ -7236,7 +7240,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>233</v>
       </c>
@@ -7259,7 +7263,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>233</v>
       </c>
@@ -7282,7 +7286,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>233</v>
       </c>
@@ -7305,7 +7309,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>233</v>
       </c>
@@ -7328,7 +7332,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>233</v>
       </c>
@@ -7351,7 +7355,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>233</v>
       </c>
@@ -7374,7 +7378,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>233</v>
       </c>
@@ -7397,7 +7401,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -7420,7 +7424,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -7443,7 +7447,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>233</v>
       </c>
@@ -7466,7 +7470,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>233</v>
       </c>
@@ -7489,7 +7493,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>233</v>
       </c>
@@ -7512,7 +7516,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>233</v>
       </c>
@@ -7535,7 +7539,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>233</v>
       </c>
@@ -7558,7 +7562,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>233</v>
       </c>
@@ -7581,7 +7585,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>233</v>
       </c>
@@ -8087,7 +8091,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="264" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>379</v>
       </c>
@@ -8110,7 +8114,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>379</v>
       </c>
@@ -8133,7 +8137,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="266" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>379</v>
       </c>
@@ -8156,7 +8160,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="267" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>379</v>
       </c>
@@ -8179,7 +8183,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>379</v>
       </c>
@@ -8202,7 +8206,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>379</v>
       </c>
@@ -8225,7 +8229,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>379</v>
       </c>
@@ -8248,7 +8252,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>379</v>
       </c>
@@ -8271,7 +8275,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>379</v>
       </c>
@@ -8294,7 +8298,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="273" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>381</v>
       </c>
@@ -8317,7 +8321,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="274" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>381</v>
       </c>
@@ -8340,7 +8344,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="275" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>381</v>
       </c>
@@ -8363,7 +8367,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="276" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>381</v>
       </c>
@@ -8386,7 +8390,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="277" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>381</v>
       </c>
@@ -8409,7 +8413,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="278" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>381</v>
       </c>
@@ -8432,7 +8436,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="279" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>381</v>
       </c>
@@ -8455,7 +8459,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="280" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>381</v>
       </c>
@@ -8478,7 +8482,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="281" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>381</v>
       </c>
@@ -8501,7 +8505,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="282" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>381</v>
       </c>
@@ -8524,7 +8528,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="283" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>381</v>
       </c>
@@ -8547,7 +8551,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="284" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>381</v>
       </c>
@@ -8570,7 +8574,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="285" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>381</v>
       </c>
@@ -8593,7 +8597,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="286" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>381</v>
       </c>
@@ -8616,7 +8620,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="287" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>381</v>
       </c>
@@ -8639,7 +8643,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="288" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>381</v>
       </c>
@@ -8662,7 +8666,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="289" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>381</v>
       </c>
@@ -8685,7 +8689,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="290" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>381</v>
       </c>
@@ -8708,7 +8712,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="291" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>381</v>
       </c>
@@ -8731,7 +8735,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="292" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>381</v>
       </c>
@@ -8754,7 +8758,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="293" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>381</v>
       </c>
@@ -8777,7 +8781,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="294" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>381</v>
       </c>
@@ -8800,7 +8804,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="295" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>381</v>
       </c>
@@ -8823,7 +8827,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="296" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>381</v>
       </c>
@@ -8846,7 +8850,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="297" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>381</v>
       </c>
@@ -8869,7 +8873,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="298" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>381</v>
       </c>
@@ -8892,7 +8896,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="299" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>381</v>
       </c>
@@ -8915,7 +8919,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="300" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>381</v>
       </c>
@@ -8938,7 +8942,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="301" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>381</v>
       </c>
@@ -8961,7 +8965,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="302" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>381</v>
       </c>
@@ -8984,7 +8988,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>381</v>
       </c>
@@ -9007,7 +9011,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="304" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>381</v>
       </c>
@@ -9030,7 +9034,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>227</v>
       </c>
@@ -9053,7 +9057,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="306" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>227</v>
       </c>
@@ -9076,7 +9080,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>227</v>
       </c>
@@ -9099,7 +9103,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="308" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>227</v>
       </c>
@@ -9122,7 +9126,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="309" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>227</v>
       </c>
@@ -9145,7 +9149,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>227</v>
       </c>
@@ -9168,7 +9172,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>227</v>
       </c>
@@ -9191,7 +9195,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>227</v>
       </c>
@@ -9214,7 +9218,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="313" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>227</v>
       </c>
@@ -9237,7 +9241,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>227</v>
       </c>
@@ -9260,7 +9264,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>227</v>
       </c>
@@ -9283,7 +9287,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>227</v>
       </c>
@@ -9306,7 +9310,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>227</v>
       </c>
@@ -9329,7 +9333,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="318" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>227</v>
       </c>
@@ -9352,7 +9356,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>227</v>
       </c>
@@ -9375,7 +9379,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>227</v>
       </c>
@@ -9398,7 +9402,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="321" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>381</v>
       </c>
@@ -9421,7 +9425,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="322" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>381</v>
       </c>
@@ -9444,7 +9448,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>381</v>
       </c>
@@ -9467,7 +9471,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>381</v>
       </c>
@@ -9490,7 +9494,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>381</v>
       </c>
@@ -9513,7 +9517,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="326" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>227</v>
       </c>
@@ -9536,7 +9540,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="327" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>227</v>
       </c>
@@ -9559,7 +9563,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="328" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>227</v>
       </c>
@@ -9582,7 +9586,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="329" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>227</v>
       </c>
@@ -9605,7 +9609,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="330" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>227</v>
       </c>
@@ -9628,7 +9632,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="331" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>240</v>
       </c>
@@ -9651,7 +9655,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="332" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>240</v>
       </c>
@@ -9674,7 +9678,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="333" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>240</v>
       </c>
@@ -9697,7 +9701,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="334" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>240</v>
       </c>
@@ -9720,7 +9724,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="335" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>240</v>
       </c>
@@ -9743,7 +9747,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="336" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>240</v>
       </c>
@@ -9766,7 +9770,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="337" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>240</v>
       </c>
@@ -9789,7 +9793,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="338" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>240</v>
       </c>
@@ -9812,7 +9816,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="339" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>240</v>
       </c>
@@ -9835,7 +9839,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="340" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>240</v>
       </c>
@@ -9858,7 +9862,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>240</v>
       </c>
@@ -9881,7 +9885,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="342" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>240</v>
       </c>
@@ -9904,7 +9908,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="343" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>240</v>
       </c>
@@ -9927,7 +9931,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="344" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>240</v>
       </c>
@@ -9950,7 +9954,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="345" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>240</v>
       </c>
@@ -9973,7 +9977,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="346" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>240</v>
       </c>
@@ -9996,7 +10000,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="347" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>240</v>
       </c>
@@ -10019,7 +10023,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="348" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>240</v>
       </c>
@@ -10042,7 +10046,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="349" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>240</v>
       </c>
@@ -10065,7 +10069,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>240</v>
       </c>
@@ -10088,7 +10092,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="351" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>240</v>
       </c>
@@ -10111,7 +10115,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="352" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>240</v>
       </c>
@@ -10134,7 +10138,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="353" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>240</v>
       </c>
@@ -10157,7 +10161,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>240</v>
       </c>
@@ -10180,7 +10184,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="355" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>240</v>
       </c>
@@ -10203,7 +10207,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="356" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>240</v>
       </c>
@@ -10226,7 +10230,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="357" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>240</v>
       </c>
@@ -10249,7 +10253,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="358" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>240</v>
       </c>
@@ -10272,7 +10276,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="359" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>240</v>
       </c>
@@ -10295,7 +10299,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="360" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>240</v>
       </c>
@@ -10318,7 +10322,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="361" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>240</v>
       </c>
@@ -10341,7 +10345,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="362" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>240</v>
       </c>
@@ -10364,7 +10368,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="363" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>240</v>
       </c>
@@ -10387,7 +10391,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="364" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>240</v>
       </c>
@@ -10410,7 +10414,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="365" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>240</v>
       </c>
@@ -10433,7 +10437,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="366" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>227</v>
       </c>
@@ -10456,7 +10460,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="367" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>227</v>
       </c>
@@ -10479,7 +10483,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="368" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>227</v>
       </c>
@@ -10502,7 +10506,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>227</v>
       </c>
@@ -10525,7 +10529,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="370" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>227</v>
       </c>
@@ -10548,7 +10552,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="371" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>227</v>
       </c>
@@ -10571,7 +10575,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="372" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>227</v>
       </c>
@@ -10594,7 +10598,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="373" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>227</v>
       </c>
@@ -10617,7 +10621,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>227</v>
       </c>
@@ -10640,7 +10644,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="375" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>227</v>
       </c>
@@ -10663,7 +10667,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>227</v>
       </c>
@@ -10686,7 +10690,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="377" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>240</v>
       </c>
@@ -10709,7 +10713,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="378" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>240</v>
       </c>
@@ -10732,7 +10736,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="379" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>240</v>
       </c>
@@ -10755,7 +10759,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="380" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>240</v>
       </c>
@@ -10778,7 +10782,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="381" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>381</v>
       </c>
@@ -10801,7 +10805,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="382" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>381</v>
       </c>
@@ -10824,7 +10828,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="383" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>381</v>
       </c>
@@ -10847,7 +10851,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="384" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>381</v>
       </c>
@@ -10870,7 +10874,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="385" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>381</v>
       </c>
@@ -10893,7 +10897,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="386" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>381</v>
       </c>
@@ -10916,7 +10920,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="387" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>381</v>
       </c>
@@ -10939,7 +10943,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="388" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>381</v>
       </c>
@@ -10962,7 +10966,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="389" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>299</v>
       </c>
@@ -10985,7 +10989,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="390" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>299</v>
       </c>
@@ -11008,7 +11012,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>299</v>
       </c>
@@ -11031,7 +11035,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="392" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>299</v>
       </c>
@@ -11054,7 +11058,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="393" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>299</v>
       </c>
@@ -11077,7 +11081,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="394" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>299</v>
       </c>
@@ -11100,7 +11104,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="395" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>299</v>
       </c>
@@ -11123,7 +11127,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="396" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>299</v>
       </c>
@@ -11146,7 +11150,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="397" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>240</v>
       </c>
@@ -11169,7 +11173,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="398" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>240</v>
       </c>
@@ -11192,7 +11196,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="399" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>240</v>
       </c>
@@ -11215,7 +11219,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="400" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>240</v>
       </c>
@@ -11238,7 +11242,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="401" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>240</v>
       </c>
@@ -11261,7 +11265,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="402" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>240</v>
       </c>
@@ -11284,7 +11288,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="403" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>240</v>
       </c>
@@ -11307,7 +11311,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="404" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>240</v>
       </c>
@@ -11330,7 +11334,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="405" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>240</v>
       </c>
@@ -11353,7 +11357,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="406" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>240</v>
       </c>
@@ -11376,7 +11380,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="407" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>240</v>
       </c>
@@ -11399,7 +11403,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="408" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>240</v>
       </c>
@@ -11422,7 +11426,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="409" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>240</v>
       </c>
@@ -11445,7 +11449,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="410" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>240</v>
       </c>
@@ -11468,7 +11472,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="411" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>240</v>
       </c>
@@ -11491,7 +11495,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="412" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>240</v>
       </c>
@@ -11514,7 +11518,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="413" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>240</v>
       </c>
@@ -11537,7 +11541,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="414" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>240</v>
       </c>
@@ -11560,7 +11564,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="415" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>240</v>
       </c>
@@ -11583,7 +11587,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="416" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>240</v>
       </c>
@@ -11606,7 +11610,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="417" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>240</v>
       </c>
@@ -11629,7 +11633,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="418" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>240</v>
       </c>
@@ -11652,7 +11656,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="419" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>240</v>
       </c>
@@ -11675,7 +11679,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="420" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>123</v>
       </c>
@@ -11698,7 +11702,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="421" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>123</v>
       </c>
@@ -11721,7 +11725,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="422" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>123</v>
       </c>
@@ -11744,7 +11748,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="423" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>123</v>
       </c>
@@ -11767,7 +11771,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="424" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>123</v>
       </c>
@@ -11790,7 +11794,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="425" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>123</v>
       </c>
@@ -11813,7 +11817,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="426" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>240</v>
       </c>
@@ -11836,7 +11840,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="427" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>240</v>
       </c>
@@ -11859,7 +11863,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="428" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>240</v>
       </c>
@@ -11882,7 +11886,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="429" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>240</v>
       </c>
@@ -11905,7 +11909,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="430" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>240</v>
       </c>
@@ -11928,7 +11932,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="431" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>239</v>
       </c>
@@ -11951,7 +11955,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="432" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>239</v>
       </c>
@@ -11974,7 +11978,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="433" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>239</v>
       </c>
@@ -11997,7 +12001,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="434" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>239</v>
       </c>
@@ -12020,7 +12024,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="435" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>240</v>
       </c>
@@ -12043,7 +12047,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="436" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>240</v>
       </c>
@@ -12066,7 +12070,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="437" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>240</v>
       </c>
@@ -12089,7 +12093,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="438" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>240</v>
       </c>
@@ -12112,7 +12116,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="439" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>240</v>
       </c>
@@ -12135,7 +12139,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="440" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>381</v>
       </c>
@@ -12158,7 +12162,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="441" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>381</v>
       </c>
@@ -12181,7 +12185,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="442" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>381</v>
       </c>
@@ -12204,7 +12208,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="443" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>381</v>
       </c>
@@ -12227,7 +12231,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="444" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>381</v>
       </c>
@@ -12250,7 +12254,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="445" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>381</v>
       </c>
@@ -12273,7 +12277,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="446" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>299</v>
       </c>
@@ -12296,7 +12300,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="447" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>299</v>
       </c>
@@ -12319,7 +12323,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="448" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>299</v>
       </c>
@@ -12342,7 +12346,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="449" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>381</v>
       </c>
@@ -12365,7 +12369,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="450" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>381</v>
       </c>
@@ -12388,7 +12392,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="451" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>381</v>
       </c>
@@ -12411,7 +12415,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="452" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>381</v>
       </c>
@@ -12434,7 +12438,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="453" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>381</v>
       </c>
@@ -12457,7 +12461,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="454" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>381</v>
       </c>
@@ -12480,7 +12484,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="455" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>381</v>
       </c>
@@ -12503,7 +12507,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="456" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>381</v>
       </c>
@@ -12526,7 +12530,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="457" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>381</v>
       </c>
@@ -12549,7 +12553,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="458" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>381</v>
       </c>
@@ -12572,7 +12576,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="459" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>381</v>
       </c>
@@ -12595,7 +12599,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="460" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>381</v>
       </c>
@@ -12618,7 +12622,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="461" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>381</v>
       </c>
@@ -12641,7 +12645,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="462" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>381</v>
       </c>
@@ -12664,7 +12668,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="463" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>381</v>
       </c>
@@ -12687,7 +12691,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="464" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>381</v>
       </c>
@@ -12710,7 +12714,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="465" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>381</v>
       </c>
@@ -12733,7 +12737,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="466" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>311</v>
       </c>
@@ -12756,7 +12760,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="467" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>311</v>
       </c>
@@ -12779,7 +12783,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="468" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>311</v>
       </c>
@@ -12802,7 +12806,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="469" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>311</v>
       </c>
@@ -12825,7 +12829,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="470" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>311</v>
       </c>
@@ -12848,7 +12852,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="471" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>311</v>
       </c>
@@ -12871,7 +12875,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="472" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>311</v>
       </c>
@@ -12894,7 +12898,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="473" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>311</v>
       </c>
@@ -12917,7 +12921,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="474" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>311</v>
       </c>
@@ -12940,7 +12944,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="475" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>311</v>
       </c>
@@ -12963,7 +12967,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="476" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>311</v>
       </c>
@@ -12986,7 +12990,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="477" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>311</v>
       </c>
@@ -13009,7 +13013,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="478" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>311</v>
       </c>
@@ -13032,7 +13036,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="479" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>311</v>
       </c>
@@ -13055,7 +13059,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="480" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>311</v>
       </c>
@@ -13078,7 +13082,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="481" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>311</v>
       </c>
@@ -13101,7 +13105,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="482" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>311</v>
       </c>
@@ -13124,7 +13128,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="483" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>311</v>
       </c>
@@ -13147,7 +13151,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="484" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>311</v>
       </c>
@@ -13170,7 +13174,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="485" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>311</v>
       </c>
@@ -13194,6 +13198,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="E1:F485">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Admin Connect"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>